<commit_message>
Atualiza dados da especificação recursos vale
</commit_message>
<xml_diff>
--- a/espec018_recursos-acordo-judicial-vale/static/template.xlsx
+++ b/espec018_recursos-acordo-judicial-vale/static/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\1. CGE\tele-trabalho\GIT\transparencia-mg\especificacoes-portal-transparencia\espec018_recursos-acordo-judicial-vale\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F7CF51-A2AD-42F0-99C7-116708DC631C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B94FBB9-ADDA-4D69-900A-AA4FE610C376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="747" firstSheet="8" activeTab="8" xr2:uid="{328BC6C1-A837-4E1A-84D5-A57C42EC6B10}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="747" firstSheet="3" activeTab="8" xr2:uid="{328BC6C1-A837-4E1A-84D5-A57C42EC6B10}"/>
   </bookViews>
   <sheets>
     <sheet name="barra- vc esta aqui" sheetId="15" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="153">
   <si>
     <t>Órgão </t>
   </si>
@@ -244,9 +244,6 @@
   </si>
   <si>
     <t>Link para o número do Empenho com o formulário</t>
-  </si>
-  <si>
-    <t>Valor Dotação Atualizada (Crédito Autorizado)</t>
   </si>
   <si>
     <t>Ano</t>
@@ -903,20 +900,6 @@
     <t>Situação da Ordem de Pagamento:</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Número Processo Compra SIAD:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1250071 000063/2021</t>
-    </r>
-  </si>
-  <si>
     <t>Dados do Processo de Compra</t>
   </si>
   <si>
@@ -1004,7 +987,160 @@
     </r>
   </si>
   <si>
-    <t>Dados do Convênio de Saída / Parceria de Recursos</t>
+    <t>Dados do Convênio  / Parceria de Saída Recursos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Título do Convênio / Parceria: :
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Data Publicação:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>26/08/2021</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Vigência Atualizada:
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Situação do Convênio / Parceria:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>xxxxxx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Número Processo Compra SIAD:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1250071 000063/2021</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Número do Convênio / Parceria SIAFI:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>xxxxxxx</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.transparencia.mg.gov.br/despesa-estado/restos-a-pagar/restospagar-orgaos/2021/4175/459/40/21/2611/130/58/2111488</t>
+  </si>
+  <si>
+    <t>Inscrição em Restos a Pagar</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tipo: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Inscrição em restos a pagar não processado</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Data de Registro: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+08/01/2021</t>
+    </r>
+  </si>
+  <si>
+    <t>Valor Inscrito:</t>
+  </si>
+  <si>
+    <t>Liquidação em Restos a Pagar</t>
+  </si>
+  <si>
+    <t>Valor Pago em Restos a Pagar</t>
+  </si>
+  <si>
+    <t>Crédito Inicial</t>
+  </si>
+  <si>
+    <t>Credito Atualizado</t>
+  </si>
+  <si>
+    <t>Liquidação e Pagamento</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1152,7 @@
     <numFmt numFmtId="164" formatCode="mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1192,6 +1328,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1231,7 +1374,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1602,13 +1745,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1703,6 +1866,15 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -1784,55 +1956,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1844,18 +1974,65 @@
     <xf numFmtId="0" fontId="25" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -5278,14 +5455,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>76202</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>66677</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>646500</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5300,7 +5477,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="581025" y="10296527"/>
+          <a:off x="581025" y="11925302"/>
           <a:ext cx="1980000" cy="285748"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -5458,13 +5635,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>707581</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>412081</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>176025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5638,13 +5815,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>453605</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>85727</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>300980</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5810,13 +5987,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>352424</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2152424</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>180973</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5987,13 +6164,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2190750</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6164,14 +6341,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>76202</xdr:rowOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>133352</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6186,7 +6363,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="581025" y="12506327"/>
+          <a:off x="581025" y="14201777"/>
           <a:ext cx="1962150" cy="285748"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -6344,13 +6521,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>695326</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>142876</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6524,13 +6701,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>205955</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>85727</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6704,13 +6881,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1860970</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>180973</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6876,13 +7053,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1895475</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1200150</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7052,15 +7229,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>76202</xdr:rowOff>
+      <xdr:colOff>549275</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>23285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1790700</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>264584</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7075,8 +7252,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="581025" y="12506327"/>
-          <a:ext cx="1819275" cy="285748"/>
+          <a:off x="549275" y="18057285"/>
+          <a:ext cx="1948392" cy="285748"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -7231,16 +7408,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1850582</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>349251</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>166500</xdr:rowOff>
+      <xdr:colOff>1873251</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>148167</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7255,8 +7432,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2460182" y="12506325"/>
-          <a:ext cx="1187893" cy="280800"/>
+          <a:off x="2582334" y="18078450"/>
+          <a:ext cx="1524000" cy="294217"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -7412,15 +7589,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1025105</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>76202</xdr:rowOff>
+      <xdr:colOff>1956438</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>65618</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>1693333</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>160866</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7435,7 +7612,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3711155" y="12506327"/>
+          <a:off x="4189521" y="18099618"/>
           <a:ext cx="1832395" cy="285748"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -7591,15 +7768,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>120647</xdr:colOff>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>584620</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:colOff>1621784</xdr:colOff>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>171448</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7615,8 +7792,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5600700" y="12506325"/>
-          <a:ext cx="1718095" cy="285748"/>
+          <a:off x="6184897" y="18110200"/>
+          <a:ext cx="1501137" cy="285748"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -7772,14 +7949,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:colOff>1804457</xdr:colOff>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2714625</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1105957</xdr:colOff>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7795,7 +7972,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7353300" y="12506325"/>
+          <a:off x="7868707" y="18110200"/>
           <a:ext cx="2095500" cy="276225"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -8115,15 +8292,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1276351</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:colOff>1371601</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>149226</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>161926</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>371476</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1562101</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>339726</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8153,7 +8330,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm rot="20914731">
-          <a:off x="1885951" y="15354301"/>
+          <a:off x="1985434" y="19326226"/>
           <a:ext cx="190500" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8176,17 +8353,17 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1276351</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:colOff>619126</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>171452</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="190500" cy="190500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="Imagem 36" descr="Ícone de lupa vermelho (símbolo png)">
+        <xdr:cNvPr id="34" name="Imagem 33" descr="Ícone de lupa vermelho (símbolo png)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFBD8BF4-158F-488A-A5C0-53488FA18201}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C0C7C98-2549-47BD-9880-135D2171A58F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8209,7 +8386,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm rot="20914731">
-          <a:off x="1885951" y="17211676"/>
+          <a:off x="1228726" y="17002127"/>
           <a:ext cx="190500" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -29662,7 +29839,7 @@
   <sheetData>
     <row r="6" spans="2:2">
       <c r="B6" s="42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -29674,15 +29851,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD08F022-29E7-400F-9167-D99313174557}">
-  <dimension ref="B4:H60"/>
+  <dimension ref="B4:H75"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="B16:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
     <col min="3" max="3" width="31.42578125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="41.85546875" customWidth="1"/>
@@ -29691,341 +29868,453 @@
   <sheetData>
     <row r="4" spans="2:8">
       <c r="H4" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="35.1" customHeight="1">
+      <c r="B6" s="96" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="H6" s="18" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="35.1" customHeight="1">
-      <c r="B6" s="73" t="s">
-        <v>101</v>
+    <row r="7" spans="2:8" ht="35.1" customHeight="1">
+      <c r="B7" s="96" t="s">
+        <v>103</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73" t="s">
+      <c r="C7" s="96"/>
+      <c r="D7" s="96" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="H6" s="18" t="s">
-        <v>100</v>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+    </row>
+    <row r="8" spans="2:8" ht="35.1" customHeight="1">
+      <c r="B8" s="96" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="H8" s="18" t="s">
+        <v>143</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="35.1" customHeight="1">
-      <c r="B7" s="73" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-    </row>
-    <row r="8" spans="2:8" ht="35.1" customHeight="1">
-      <c r="B8" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73" t="s">
+    <row r="9" spans="2:8" ht="35.1" customHeight="1">
+      <c r="B9" s="96" t="s">
         <v>106</v>
       </c>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-    </row>
-    <row r="9" spans="2:8" ht="35.1" customHeight="1">
-      <c r="B9" s="73" t="s">
+      <c r="C9" s="96"/>
+      <c r="D9" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73" t="s">
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+    </row>
+    <row r="10" spans="2:8" ht="35.1" customHeight="1">
+      <c r="B10" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
     </row>
-    <row r="10" spans="2:8" ht="35.1" customHeight="1">
-      <c r="B10" s="73" t="s">
+    <row r="11" spans="2:8" ht="35.1" customHeight="1">
+      <c r="B11" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73" t="s">
+      <c r="C11" s="96"/>
+      <c r="D11" s="96" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
     </row>
-    <row r="11" spans="2:8" ht="35.1" customHeight="1">
-      <c r="B11" s="73" t="s">
+    <row r="12" spans="2:8" ht="41.25" customHeight="1">
+      <c r="B12" s="96" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73" t="s">
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="96"/>
+    </row>
+    <row r="19" spans="2:5" ht="35.1" customHeight="1">
+      <c r="B19" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-    </row>
-    <row r="12" spans="2:8" ht="41.25" customHeight="1">
-      <c r="B12" s="73" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
     </row>
     <row r="20" spans="2:5" ht="35.1" customHeight="1">
-      <c r="B20" s="74" t="s">
-        <v>115</v>
+      <c r="B20" s="92" t="s">
+        <v>127</v>
       </c>
-      <c r="C20" s="74" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="74" t="s">
+      <c r="C20" s="93"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="94"/>
+    </row>
+    <row r="21" spans="2:5" ht="35.1" customHeight="1">
+      <c r="B21" s="92" t="s">
         <v>117</v>
       </c>
-      <c r="E20" s="74" t="s">
-        <v>114</v>
+      <c r="C21" s="93"/>
+      <c r="D21" s="92" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="94"/>
+    </row>
+    <row r="22" spans="2:5" ht="30.75" customHeight="1">
+      <c r="B22" s="92" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="93"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="94"/>
+    </row>
+    <row r="23" spans="2:5" ht="26.25" customHeight="1">
+      <c r="B23" s="95" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+    </row>
+    <row r="24" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B24" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="82" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="84"/>
+    </row>
+    <row r="25" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="84"/>
+    </row>
+    <row r="26" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B26" s="89" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="91"/>
+    </row>
+    <row r="27" spans="2:5" ht="35.1" customHeight="1">
+      <c r="B27" s="95" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+    </row>
+    <row r="28" spans="2:5" ht="20.25" customHeight="1">
+      <c r="B28" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="82" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" s="84"/>
+    </row>
+    <row r="29" spans="2:5" ht="18.75" customHeight="1">
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="84"/>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="89" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="91"/>
+    </row>
+    <row r="32" spans="2:5" ht="27" customHeight="1">
+      <c r="B32" s="97" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" s="98"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
+    </row>
+    <row r="33" spans="2:6" ht="38.25" customHeight="1">
+      <c r="B33" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="92" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" s="94"/>
+      <c r="E33" s="46" t="s">
+        <v>147</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="35.1" customHeight="1">
-      <c r="B21" s="75" t="s">
+    <row r="40" spans="2:6" ht="34.5" customHeight="1"/>
+    <row r="41" spans="2:6">
+      <c r="B41" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="E41" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="76"/>
+      <c r="F41" s="48" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="22" spans="2:5" ht="35.1" customHeight="1">
-      <c r="B22" s="75" t="s">
-        <v>118</v>
+    <row r="42" spans="2:6">
+      <c r="B42" s="47"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+    </row>
+    <row r="43" spans="2:6" ht="19.5" customHeight="1">
+      <c r="B43" s="47"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="89" t="s">
+        <v>129</v>
       </c>
-      <c r="C22" s="77"/>
-      <c r="D22" s="75" t="s">
+      <c r="C44" s="90"/>
+      <c r="D44" s="90"/>
+      <c r="E44" s="91"/>
+      <c r="F44" s="46"/>
+    </row>
+    <row r="46" spans="2:6" ht="24.75" customHeight="1">
+      <c r="B46" s="99" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" s="100"/>
+      <c r="D46" s="100"/>
+      <c r="E46" s="100"/>
+      <c r="F46" s="100"/>
+    </row>
+    <row r="47" spans="2:6" ht="29.25" customHeight="1">
+      <c r="B47" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="47" t="s">
         <v>120</v>
       </c>
-      <c r="E22" s="76"/>
-    </row>
-    <row r="23" spans="2:5" ht="98.25" customHeight="1">
-      <c r="B23" s="75" t="s">
-        <v>119</v>
+      <c r="D47" s="47" t="s">
+        <v>126</v>
       </c>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="76"/>
-    </row>
-    <row r="24" spans="2:5" ht="26.25" customHeight="1">
-      <c r="B24" s="79" t="s">
-        <v>124</v>
+      <c r="E47" s="48" t="s">
+        <v>128</v>
       </c>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-    </row>
-    <row r="25" spans="2:5" ht="35.1" customHeight="1">
-      <c r="B25" s="78" t="s">
+      <c r="F47" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="78" t="s">
-        <v>121</v>
-      </c>
-      <c r="D25" s="80" t="s">
-        <v>123</v>
-      </c>
-      <c r="E25" s="81"/>
     </row>
-    <row r="26" spans="2:5" ht="35.1" customHeight="1">
-      <c r="B26" s="79" t="s">
+    <row r="48" spans="2:6" ht="20.25" customHeight="1">
+      <c r="B48" s="47"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+    </row>
+    <row r="55" spans="2:6" ht="25.5">
+      <c r="B55" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="79"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
-    </row>
-    <row r="27" spans="2:5" ht="35.1" customHeight="1">
-      <c r="B27" s="78" t="s">
+      <c r="C55" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="F55" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="78" t="s">
-        <v>121</v>
-      </c>
-      <c r="D27" s="80" t="s">
-        <v>123</v>
-      </c>
-      <c r="E27" s="81"/>
     </row>
-    <row r="34" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B34" s="78" t="s">
-        <v>126</v>
-      </c>
-      <c r="C34" s="78" t="s">
-        <v>121</v>
-      </c>
-      <c r="D34" s="78" t="s">
-        <v>127</v>
-      </c>
-      <c r="E34" s="82" t="s">
+    <row r="56" spans="2:6">
+      <c r="B56" s="47"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46"/>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57" s="47"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="B58" s="89" t="s">
         <v>129</v>
       </c>
-      <c r="F34" s="82" t="s">
-        <v>123</v>
+      <c r="C58" s="90"/>
+      <c r="D58" s="90"/>
+      <c r="E58" s="91"/>
+      <c r="F58" s="46"/>
+    </row>
+    <row r="60" spans="2:6">
+      <c r="B60" s="99" t="s">
+        <v>149</v>
+      </c>
+      <c r="C60" s="100"/>
+      <c r="D60" s="100"/>
+      <c r="E60" s="100"/>
+      <c r="F60" s="100"/>
+    </row>
+    <row r="61" spans="2:6" ht="33" customHeight="1">
+      <c r="B61" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="E61" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="F61" s="48" t="s">
+        <v>122</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
-      <c r="B35" s="78"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="74"/>
-      <c r="F35" s="74"/>
-    </row>
-    <row r="36" spans="2:6">
-      <c r="B36" s="78"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-    </row>
-    <row r="37" spans="2:6" ht="19.5" customHeight="1">
-      <c r="B37" s="86" t="s">
-        <v>130</v>
-      </c>
-      <c r="C37" s="87"/>
-      <c r="D37" s="87"/>
-      <c r="E37" s="88"/>
-      <c r="F37" s="74"/>
-    </row>
-    <row r="44" spans="2:6" ht="25.5">
-      <c r="B44" s="78" t="s">
-        <v>126</v>
-      </c>
-      <c r="C44" s="78" t="s">
-        <v>121</v>
-      </c>
-      <c r="D44" s="78" t="s">
+    <row r="66" spans="2:6" ht="25.5" customHeight="1"/>
+    <row r="67" spans="2:6" ht="34.5" customHeight="1">
+      <c r="B67" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="E44" s="82" t="s">
-        <v>129</v>
+      <c r="C67" s="80"/>
+      <c r="D67" s="80"/>
+      <c r="E67" s="80"/>
+      <c r="F67" s="81"/>
+    </row>
+    <row r="68" spans="2:6" ht="40.5" customHeight="1">
+      <c r="B68" s="82" t="s">
+        <v>141</v>
       </c>
-      <c r="F44" s="82" t="s">
-        <v>123</v>
+      <c r="C68" s="83"/>
+      <c r="D68" s="84"/>
+      <c r="E68" s="82" t="s">
+        <v>132</v>
       </c>
+      <c r="F68" s="84"/>
     </row>
-    <row r="45" spans="2:6">
-      <c r="B45" s="78"/>
-      <c r="C45" s="78"/>
-      <c r="D45" s="78"/>
-      <c r="E45" s="74"/>
-      <c r="F45" s="74"/>
+    <row r="69" spans="2:6" ht="40.5" customHeight="1">
+      <c r="B69" s="85" t="s">
+        <v>134</v>
+      </c>
+      <c r="C69" s="86"/>
+      <c r="D69" s="87"/>
+      <c r="E69" s="77" t="s">
+        <v>135</v>
+      </c>
+      <c r="F69" s="88"/>
     </row>
-    <row r="46" spans="2:6">
-      <c r="B46" s="78"/>
-      <c r="C46" s="78"/>
-      <c r="D46" s="78"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="74"/>
-    </row>
-    <row r="47" spans="2:6">
-      <c r="B47" s="86" t="s">
-        <v>130</v>
-      </c>
-      <c r="C47" s="87"/>
-      <c r="D47" s="87"/>
-      <c r="E47" s="88"/>
-      <c r="F47" s="74"/>
-    </row>
-    <row r="53" spans="2:6" ht="25.5" customHeight="1">
-      <c r="B53" s="90" t="s">
+    <row r="70" spans="2:6">
+      <c r="B70" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="C53" s="91"/>
-      <c r="D53" s="91"/>
-      <c r="E53" s="91"/>
-      <c r="F53" s="92"/>
+      <c r="C70" s="77"/>
+      <c r="D70" s="77"/>
+      <c r="E70" s="77"/>
+      <c r="F70" s="78"/>
     </row>
-    <row r="54" spans="2:6" ht="34.5" customHeight="1">
-      <c r="B54" s="80" t="s">
-        <v>132</v>
-      </c>
-      <c r="C54" s="89"/>
-      <c r="D54" s="81"/>
-      <c r="E54" s="80" t="s">
-        <v>134</v>
-      </c>
-      <c r="F54" s="81"/>
-    </row>
-    <row r="55" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B55" s="83" t="s">
+    <row r="71" spans="2:6" ht="28.5" customHeight="1">
+      <c r="B71" s="79" t="s">
         <v>136</v>
       </c>
-      <c r="C55" s="84"/>
-      <c r="D55" s="85"/>
-      <c r="E55" s="93" t="s">
+      <c r="C71" s="80"/>
+      <c r="D71" s="80"/>
+      <c r="E71" s="80"/>
+      <c r="F71" s="81"/>
+    </row>
+    <row r="72" spans="2:6" ht="28.5" customHeight="1">
+      <c r="B72" s="82" t="s">
+        <v>142</v>
+      </c>
+      <c r="C72" s="83"/>
+      <c r="D72" s="84"/>
+      <c r="E72" s="82" t="s">
+        <v>138</v>
+      </c>
+      <c r="F72" s="84"/>
+    </row>
+    <row r="73" spans="2:6" ht="47.25" customHeight="1">
+      <c r="B73" s="85" t="s">
+        <v>140</v>
+      </c>
+      <c r="C73" s="86"/>
+      <c r="D73" s="87"/>
+      <c r="E73" s="77" t="s">
+        <v>139</v>
+      </c>
+      <c r="F73" s="88"/>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="B74" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="F55" s="96"/>
+      <c r="C74" s="77"/>
+      <c r="D74" s="77"/>
+      <c r="E74" s="77"/>
+      <c r="F74" s="78"/>
     </row>
-    <row r="56" spans="2:6" ht="40.5" customHeight="1">
-      <c r="B56" s="95" t="s">
-        <v>135</v>
-      </c>
-      <c r="C56" s="93"/>
-      <c r="D56" s="93"/>
-      <c r="E56" s="93"/>
-      <c r="F56" s="94"/>
-    </row>
-    <row r="57" spans="2:6">
-      <c r="B57" s="90" t="s">
-        <v>138</v>
-      </c>
-      <c r="C57" s="91"/>
-      <c r="D57" s="91"/>
-      <c r="E57" s="91"/>
-      <c r="F57" s="92"/>
-    </row>
-    <row r="58" spans="2:6" ht="28.5" customHeight="1">
-      <c r="B58" s="80"/>
-      <c r="C58" s="89"/>
-      <c r="D58" s="81"/>
-      <c r="E58" s="80"/>
-      <c r="F58" s="81"/>
-    </row>
-    <row r="59" spans="2:6" ht="28.5" customHeight="1">
-      <c r="B59" s="83"/>
-      <c r="C59" s="84"/>
-      <c r="D59" s="85"/>
-      <c r="E59" s="93"/>
-      <c r="F59" s="96"/>
-    </row>
-    <row r="60" spans="2:6" ht="28.5" customHeight="1">
-      <c r="B60" s="95"/>
-      <c r="C60" s="93"/>
-      <c r="D60" s="93"/>
-      <c r="E60" s="93"/>
-      <c r="F60" s="94"/>
-    </row>
+    <row r="75" spans="2:6" ht="22.5" customHeight="1"/>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="44">
+    <mergeCell ref="B46:F46"/>
     <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="B26:E26"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B20:E20"/>
     <mergeCell ref="B23:E23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="B7:C7"/>
@@ -30038,16 +30327,36 @@
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="E73:F73"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{1B84B5CA-5CC6-4815-96AA-B62982CE1722}"/>
     <hyperlink ref="H4" r:id="rId2" xr:uid="{0CF0A032-F03D-4D12-BE3B-1214A2D4525B}"/>
+    <hyperlink ref="H8" r:id="rId3" xr:uid="{DBED3DE1-1339-4590-9592-7C0B478A5BDB}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -30056,7 +30365,7 @@
   <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30319,36 +30628,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="18">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
+      <c r="A1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="W1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="18">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
       <c r="Q2" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W2">
         <v>2021</v>
@@ -30369,13 +30678,13 @@
     </row>
     <row r="7" spans="1:25">
       <c r="W7" t="s">
+        <v>60</v>
+      </c>
+      <c r="X7" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="X7" s="35" t="s">
+      <c r="Y7" t="s">
         <v>62</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -30391,7 +30700,7 @@
     </row>
     <row r="9" spans="1:25" ht="16.5">
       <c r="B9" s="43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="W9" s="34">
         <v>9500000</v>
@@ -30475,39 +30784,39 @@
     <row r="18" spans="1:1" ht="15" customHeight="1"/>
     <row r="25" spans="1:1">
       <c r="A25" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="39" spans="1:4">
       <c r="D39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="33" customFormat="1">
       <c r="A46" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="33" customFormat="1">
       <c r="A47" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="33" customFormat="1">
       <c r="A48" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:1" s="33" customFormat="1"/>
     <row r="50" spans="1:1" s="33" customFormat="1">
       <c r="A50" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:1" s="33" customFormat="1">
       <c r="A51" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -30540,13 +30849,13 @@
   <sheetData>
     <row r="3" spans="2:2" ht="15.75">
       <c r="B3" s="41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="2:2" ht="15" customHeight="1"/>
     <row r="18" spans="1:1">
       <c r="A18" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -30587,80 +30896,80 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" thickBot="1">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="55"/>
+      <c r="F6" s="58"/>
       <c r="H6" s="29" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" thickBot="1">
-      <c r="A7" s="56" t="s">
-        <v>72</v>
+      <c r="A7" s="59" t="s">
+        <v>71</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="63">
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="66">
         <f>'Pesquisa básica 1'!X2</f>
         <v>3478961699.73</v>
       </c>
-      <c r="F7" s="64"/>
+      <c r="F7" s="67"/>
       <c r="H7" s="30" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1">
-      <c r="A8" s="47" t="s">
-        <v>61</v>
+      <c r="A8" s="50" t="s">
+        <v>60</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="65">
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="68">
         <f>'Pesquisa básica 1'!W15</f>
         <v>720584233.74000001</v>
       </c>
-      <c r="F8" s="66"/>
+      <c r="F8" s="69"/>
       <c r="H8" s="30" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" thickBot="1">
       <c r="A9" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="69">
+      <c r="E9" s="72">
         <f>'Pesquisa básica 1'!X15</f>
         <v>599300000</v>
       </c>
-      <c r="F9" s="70"/>
+      <c r="F9" s="73"/>
       <c r="H9" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A10" s="60" t="s">
-        <v>63</v>
+      <c r="A10" s="63" t="s">
+        <v>62</v>
       </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="67">
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="70">
         <f>'Pesquisa básica 1'!Y15</f>
         <v>599300000</v>
       </c>
-      <c r="F10" s="68"/>
+      <c r="F10" s="71"/>
       <c r="H10" s="30" t="s">
         <v>49</v>
       </c>
@@ -30687,29 +30996,29 @@
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A21" s="51" t="s">
-        <v>68</v>
+      <c r="A21" s="54" t="s">
+        <v>67</v>
       </c>
-      <c r="B21" s="53"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="5">
         <v>2021</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="F21" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A22" s="56" t="str">
+      <c r="A22" s="59" t="str">
         <f>A7</f>
         <v>Repassado ao Estado</v>
       </c>
-      <c r="B22" s="58"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="13">
         <f>E7</f>
         <v>3478961699.73</v>
@@ -30719,11 +31028,11 @@
       <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A23" s="47" t="str">
+      <c r="A23" s="50" t="str">
         <f>A8</f>
         <v>Empenhado</v>
       </c>
-      <c r="B23" s="48"/>
+      <c r="B23" s="51"/>
       <c r="C23" s="3">
         <f>E8</f>
         <v>720584233.74000001</v>
@@ -30733,11 +31042,11 @@
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A24" s="47" t="str">
+      <c r="A24" s="50" t="str">
         <f>A9</f>
         <v>Liquidado</v>
       </c>
-      <c r="B24" s="48"/>
+      <c r="B24" s="51"/>
       <c r="C24" s="3">
         <f>E9</f>
         <v>599300000</v>
@@ -30747,11 +31056,11 @@
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A25" s="47" t="str">
+      <c r="A25" s="50" t="str">
         <f>A10</f>
         <v>Pago</v>
       </c>
-      <c r="B25" s="48"/>
+      <c r="B25" s="51"/>
       <c r="C25" s="3">
         <f>E10</f>
         <v>599300000</v>
@@ -30761,10 +31070,10 @@
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="50"/>
+      <c r="B26" s="53"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8">
         <f>SUM(D22:D25)</f>
@@ -30807,8 +31116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE53348-60D5-456C-BD65-114FBC69E794}">
   <dimension ref="O4:Q24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7:O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30830,129 +31139,129 @@
       </c>
     </row>
     <row r="5" spans="15:17" ht="30" customHeight="1">
-      <c r="O5" s="71" t="s">
+      <c r="O5" s="74" t="s">
+        <v>96</v>
+      </c>
+      <c r="P5" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="P5" s="71" t="s">
-        <v>98</v>
-      </c>
       <c r="Q5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="15:17">
-      <c r="O6" s="71"/>
-      <c r="P6" s="71"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="74"/>
     </row>
     <row r="7" spans="15:17">
       <c r="O7" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P7" s="45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="15:17">
       <c r="O8" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P8" s="45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="15:17">
       <c r="O9" s="44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P9" s="45"/>
     </row>
     <row r="10" spans="15:17">
       <c r="O10" s="44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P10" s="45"/>
     </row>
     <row r="11" spans="15:17">
       <c r="O11" s="44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P11" s="45"/>
     </row>
     <row r="12" spans="15:17">
       <c r="O12" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P12" s="45"/>
     </row>
     <row r="13" spans="15:17">
       <c r="O13" s="44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P13" s="45"/>
     </row>
     <row r="14" spans="15:17">
       <c r="O14" s="45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P14" s="45"/>
     </row>
     <row r="15" spans="15:17">
       <c r="O15" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P15" s="45"/>
     </row>
     <row r="16" spans="15:17">
       <c r="O16" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P16" s="45"/>
     </row>
     <row r="17" spans="15:16">
       <c r="O17" s="45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P17" s="45"/>
     </row>
     <row r="18" spans="15:16">
       <c r="O18" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P18" s="45"/>
     </row>
     <row r="19" spans="15:16">
       <c r="O19" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P19" s="45"/>
     </row>
     <row r="20" spans="15:16">
       <c r="O20" s="45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P20" s="45"/>
     </row>
     <row r="21" spans="15:16">
       <c r="O21" s="45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P21" s="45"/>
     </row>
     <row r="22" spans="15:16">
       <c r="O22" s="45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P22" s="45"/>
     </row>
     <row r="23" spans="15:16">
       <c r="O23" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P23" s="45"/>
     </row>
     <row r="24" spans="15:16">
       <c r="O24" s="45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P24" s="45"/>
     </row>
@@ -31199,11 +31508,11 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="72"/>
-      <c r="C17" s="50"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="53"/>
       <c r="D17" s="8">
         <f>SUM(D11:D16)</f>
         <v>603978445.99666667</v>
@@ -31236,10 +31545,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5105E053-53E6-452E-8454-A31AB296F312}">
-  <dimension ref="A5:H25"/>
+  <dimension ref="A4:H25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.42578125" defaultRowHeight="15"/>
@@ -31255,13 +31564,18 @@
     <col min="9" max="16384" width="76.42578125" style="1"/>
   </cols>
   <sheetData>
+    <row r="4" spans="1:8">
+      <c r="H4" s="44" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="5" spans="1:8" ht="21.75" customHeight="1" thickBot="1">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="H5" s="1" t="s">
-        <v>44</v>
+      <c r="H5" s="44" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" thickBot="1">
@@ -31283,8 +31597,8 @@
       <c r="F6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="29" t="s">
-        <v>53</v>
+      <c r="H6" s="44" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" thickBot="1">
@@ -31294,8 +31608,8 @@
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="H7" s="30" t="s">
-        <v>46</v>
+      <c r="H7" s="44" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1">
@@ -31305,8 +31619,8 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="H8" s="30" t="s">
-        <v>47</v>
+      <c r="H8" s="44" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" thickBot="1">
@@ -31316,15 +31630,15 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="H9" s="30" t="s">
-        <v>48</v>
+      <c r="H9" s="44" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="50"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8">
         <f>SUM(D7:D9)</f>
@@ -31338,32 +31652,65 @@
         <f>SUM(F7:F9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="30" t="s">
-        <v>49</v>
+      <c r="H10" s="44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="H11" s="45" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="H12" s="30" t="s">
-        <v>52</v>
+      <c r="H12" s="45" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="H13" s="30" t="s">
-        <v>50</v>
+      <c r="H13" s="45" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="H14" s="30" t="s">
-        <v>51</v>
+      <c r="H14" s="45" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1">
+    <row r="15" spans="1:8">
+      <c r="H15" s="45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="H16" s="45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="H17" s="45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="H18" s="45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="H19" s="45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
+      <c r="H20" s="45" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="21" spans="1:6" ht="24.75" customHeight="1" thickBot="1">
+    <row r="21" spans="1:8" ht="24.75" customHeight="1" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
@@ -31383,35 +31730,44 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
+    <row r="22" spans="1:8" ht="27.75" customHeight="1" thickBot="1">
       <c r="A22" s="27"/>
       <c r="B22" s="14"/>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
+      <c r="H22" s="101" t="s">
+        <v>150</v>
+      </c>
     </row>
-    <row r="23" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
+    <row r="23" spans="1:8" ht="27.75" customHeight="1" thickBot="1">
       <c r="A23" s="28"/>
       <c r="B23" s="7"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
+      <c r="H23" s="101" t="s">
+        <v>151</v>
+      </c>
     </row>
-    <row r="24" spans="1:6" ht="27.75" customHeight="1" thickBot="1">
+    <row r="24" spans="1:8" ht="27.75" customHeight="1" thickBot="1">
       <c r="A24" s="28"/>
       <c r="B24" s="7"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
+      <c r="H24" s="45" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="25" spans="1:6" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A25" s="49" t="s">
+    <row r="25" spans="1:8" ht="22.5" customHeight="1" thickBot="1">
+      <c r="A25" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="50"/>
+      <c r="B25" s="53"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8">
         <f>SUM(D22:D24)</f>
@@ -31425,6 +31781,9 @@
         <f>SUM(F22:F24)</f>
         <v>0</v>
       </c>
+      <c r="H25" s="102" t="s">
+        <v>152</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>